<commit_message>
add differenceCurrentDesiredAccounts, portfolioValue, categoryTotal functions and unit tests
</commit_message>
<xml_diff>
--- a/test/test_reallocate.xlsx
+++ b/test/test_reallocate.xlsx
@@ -651,17 +651,17 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="5" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -785,6 +785,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="4" t="n">
+        <f aca="false">SUM(E2:S2)</f>
         <v>94253</v>
       </c>
     </row>
@@ -847,6 +848,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="4" t="n">
+        <f aca="false">SUM(E3:S3)</f>
         <v>39695</v>
       </c>
     </row>
@@ -864,7 +866,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>13793.05</v>
+        <v>13793</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>1729.84</v>
@@ -909,7 +911,8 @@
         <v>0</v>
       </c>
       <c r="T4" s="4" t="n">
-        <v>28439.02</v>
+        <f aca="false">SUM(E4:S4)</f>
+        <v>48438.97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -926,7 +929,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>447.13</v>
+        <v>447</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>1096.64</v>
@@ -971,7 +974,8 @@
         <v>0</v>
       </c>
       <c r="T5" s="4" t="n">
-        <v>9413.24</v>
+        <f aca="false">SUM(E5:S5)</f>
+        <v>9413.11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -988,7 +992,7 @@
         <v>35</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>6.09</v>
+        <v>6</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>0</v>
@@ -1033,7 +1037,8 @@
         <v>0</v>
       </c>
       <c r="T6" s="4" t="n">
-        <v>5507.04</v>
+        <f aca="false">SUM(E6:S6)</f>
+        <v>5506.95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1050,7 +1055,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>79.05</v>
+        <v>79</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>0</v>
@@ -1095,7 +1100,8 @@
         <v>0</v>
       </c>
       <c r="T7" s="4" t="n">
-        <v>79054.34</v>
+        <f aca="false">SUM(E7:S7)</f>
+        <v>79054.29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1112,7 +1118,7 @@
         <v>40</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>220.99</v>
+        <v>220</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>0</v>
@@ -1157,7 +1163,8 @@
         <v>0</v>
       </c>
       <c r="T8" s="4" t="n">
-        <v>220992.1</v>
+        <f aca="false">SUM(E8:S8)</f>
+        <v>220991.11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1174,7 +1181,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>283.09</v>
+        <v>283</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>0</v>
@@ -1219,7 +1226,8 @@
         <v>0</v>
       </c>
       <c r="T9" s="4" t="n">
-        <v>2380.9</v>
+        <f aca="false">SUM(E9:S9)</f>
+        <v>2380.81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1236,7 +1244,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>54.65</v>
+        <v>54</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>0</v>
@@ -1281,7 +1289,8 @@
         <v>0</v>
       </c>
       <c r="T10" s="4" t="n">
-        <v>68382.85</v>
+        <f aca="false">SUM(E10:S10)</f>
+        <v>68382.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1343,7 +1352,8 @@
         <v>0</v>
       </c>
       <c r="T11" s="4" t="n">
-        <v>127909.33</v>
+        <f aca="false">SUM(E11:S11)</f>
+        <v>142802.78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1405,6 +1415,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="4" t="n">
+        <f aca="false">SUM(E12:S12)</f>
         <v>3522</v>
       </c>
     </row>
@@ -1467,6 +1478,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="4" t="n">
+        <f aca="false">SUM(E13:S13)</f>
         <v>28315</v>
       </c>
     </row>
@@ -1529,7 +1541,8 @@
         <v>0</v>
       </c>
       <c r="T14" s="4" t="n">
-        <v>0</v>
+        <f aca="false">SUM(E14:S14)</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1540,52 +1553,68 @@
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="6" t="n">
-        <v>112765.6</v>
-      </c>
-      <c r="F15" s="7" t="n">
+        <f aca="false">SUM(E2:E14)</f>
+        <v>112657</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <f aca="false">SUM(F2:F14)</f>
         <v>2826.48</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="6" t="n">
+        <f aca="false">SUM(G2:G14)</f>
         <v>30430.96</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="6" t="n">
+        <f aca="false">SUM(H2:H14)</f>
         <v>106256.16</v>
       </c>
-      <c r="I15" s="4" t="n">
+      <c r="I15" s="6" t="n">
+        <f aca="false">SUM(I2:I14)</f>
         <v>144848.42</v>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="6" t="n">
+        <f aca="false">SUM(J2:J14)</f>
         <v>102876.96</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="6" t="n">
+        <f aca="false">SUM(K2:K14)</f>
         <v>50071.64</v>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" s="6" t="n">
+        <f aca="false">SUM(L2:L14)</f>
         <v>43937.44</v>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="M15" s="6" t="n">
+        <f aca="false">SUM(M2:M14)</f>
         <v>25183.64</v>
       </c>
-      <c r="N15" s="4" t="n">
+      <c r="N15" s="6" t="n">
+        <f aca="false">SUM(N2:N14)</f>
         <v>43278.06</v>
       </c>
-      <c r="O15" s="4" t="n">
+      <c r="O15" s="6" t="n">
+        <f aca="false">SUM(O2:O14)</f>
         <v>33947.23</v>
       </c>
-      <c r="P15" s="4" t="n">
+      <c r="P15" s="6" t="n">
+        <f aca="false">SUM(P2:P14)</f>
         <v>6071.11</v>
       </c>
-      <c r="Q15" s="4" t="n">
+      <c r="Q15" s="6" t="n">
+        <f aca="false">SUM(Q2:Q14)</f>
         <v>5370.12</v>
       </c>
-      <c r="R15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" s="4" t="n">
-        <v>707863.82</v>
+      <c r="R15" s="6" t="n">
+        <f aca="false">SUM(R2:R14)</f>
+        <v>45000</v>
+      </c>
+      <c r="S15" s="6" t="n">
+        <f aca="false">SUM(S2:S14)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="6" t="n">
+        <f aca="false">SUM(T2:T14)</f>
+        <v>752755.22</v>
       </c>
     </row>
   </sheetData>
@@ -1615,13 +1644,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1866,7 +1895,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,12 +1959,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,10 +2361,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,11 +2486,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2614,11 +2648,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
categoryCountAs function and unit test, modified categoryRules dictionary
</commit_message>
<xml_diff>
--- a/test/test_reallocate.xlsx
+++ b/test/test_reallocate.xlsx
@@ -650,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1319,7 +1319,7 @@
         <v>11084.65</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>10838.4</v>
+        <v>838.4</v>
       </c>
       <c r="J11" s="4" t="n">
         <v>10695.17</v>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="T11" s="4" t="n">
         <f aca="false">SUM(E11:S11)</f>
-        <v>142802.78</v>
+        <v>132802.78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1538,11 +1538,11 @@
         <v>10000</v>
       </c>
       <c r="S14" s="8" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="T14" s="4" t="n">
         <f aca="false">SUM(E14:S14)</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="I15" s="6" t="n">
         <f aca="false">SUM(I2:I14)</f>
-        <v>144848.42</v>
+        <v>134848.42</v>
       </c>
       <c r="J15" s="6" t="n">
         <f aca="false">SUM(J2:J14)</f>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="S15" s="6" t="n">
         <f aca="false">SUM(S2:S14)</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="T15" s="6" t="n">
         <f aca="false">SUM(T2:T14)</f>
@@ -1639,7 +1639,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>